<commit_message>
Updated Code with AI Analyzer
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/FormFieldTestData.xlsx
+++ b/src/test/resources/testdata/FormFieldTestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -329,7 +329,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="105" x14ac:knownFonts="1">
+  <fonts count="734" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -613,6 +613,3151 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="9"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -932,7 +4077,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="741">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1065,6 +4210,635 @@
     <xf numFmtId="0" fontId="102" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="103" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="104" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="105" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="106" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="107" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="108" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="109" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="110" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="111" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="112" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="113" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="114" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="115" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="116" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="117" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="118" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="119" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="120" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="121" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="122" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="123" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="124" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="125" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="126" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="127" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="128" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="129" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="130" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="131" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="132" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="133" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="134" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="135" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="136" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="137" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="138" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="139" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="140" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="141" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="142" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="143" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="144" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="145" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="146" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="147" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="148" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="149" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="150" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="151" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="152" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="153" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="154" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="155" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="156" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="157" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="158" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="159" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="160" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="161" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="162" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="163" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="164" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="165" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="166" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="167" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="168" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="169" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="170" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="171" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="172" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="173" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="174" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="175" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="176" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="177" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="178" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="179" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="180" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="181" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="182" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="183" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="184" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="185" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="186" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="187" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="188" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="189" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="190" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="191" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="192" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="193" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="194" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="195" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="196" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="197" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="198" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="199" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="200" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="201" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="202" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="203" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="204" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="205" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="206" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="207" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="208" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="209" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="210" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="211" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="212" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="213" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="214" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="215" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="216" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="217" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="218" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="219" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="220" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="221" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="222" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="223" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="224" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="225" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="226" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="227" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="228" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="229" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="230" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="231" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="232" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="233" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="234" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="235" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="236" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="237" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="238" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="239" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="240" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="241" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="242" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="243" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="244" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="245" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="246" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="247" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="248" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="249" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="250" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="251" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="252" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="253" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="254" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="255" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="256" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="257" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="258" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="259" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="260" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="261" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="262" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="263" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="264" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="265" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="266" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="267" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="268" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="269" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="270" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="271" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="272" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="273" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="274" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="275" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="276" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="277" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="278" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="279" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="280" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="281" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="282" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="283" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="284" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="285" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="286" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="287" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="288" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="289" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="290" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="291" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="292" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="293" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="294" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="295" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="296" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="297" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="298" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="299" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="300" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="301" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="302" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="303" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="304" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="305" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="306" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="307" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="308" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="309" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="310" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="311" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="312" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="313" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="314" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="315" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="316" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="317" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="318" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="319" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="320" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="321" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="322" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="323" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="324" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="325" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="326" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="327" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="328" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="329" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="330" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="331" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="332" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="333" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="334" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="335" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="336" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="337" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="338" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="339" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="340" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="341" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="342" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="343" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="344" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="345" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="346" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="347" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="348" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="349" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="350" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="351" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="352" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="353" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="354" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="355" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="356" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="357" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="358" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="359" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="360" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="361" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="362" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="363" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="364" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="365" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="366" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="367" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="368" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="369" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="370" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="371" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="372" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="373" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="374" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="375" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="376" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="377" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="378" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="379" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="380" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="381" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="382" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="383" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="384" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="385" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="386" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="387" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="388" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="389" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="390" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="391" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="392" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="393" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="394" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="395" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="396" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="397" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="398" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="399" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="400" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="401" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="402" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="403" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="404" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="405" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="406" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="407" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="408" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="409" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="410" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="411" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="412" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="413" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="414" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="415" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="416" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="417" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="418" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="419" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="420" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="421" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="422" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="423" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="424" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="425" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="426" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="427" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="428" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="429" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="430" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="431" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="432" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="433" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="434" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="435" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="436" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="437" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="438" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="439" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="440" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="441" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="442" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="443" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="444" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="445" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="446" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="447" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="448" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="449" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="450" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="451" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="452" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="453" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="454" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="455" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="456" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="457" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="458" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="459" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="460" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="461" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="462" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="463" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="464" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="465" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="466" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="467" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="468" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="469" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="470" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="471" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="472" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="473" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="474" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="475" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="476" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="477" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="478" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="479" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="480" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="481" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="482" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="483" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="484" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="485" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="486" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="487" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="488" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="489" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="490" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="491" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="492" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="493" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="494" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="495" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="496" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="497" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="498" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="499" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="500" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="501" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="502" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="503" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="504" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="505" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="506" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="507" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="508" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="509" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="510" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="511" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="512" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="513" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="514" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="515" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="516" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="517" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="518" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="519" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="520" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="521" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="522" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="523" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="524" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="525" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="526" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="527" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="528" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="529" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="530" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="531" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="532" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="533" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="534" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="535" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="536" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="537" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="538" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="539" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="540" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="541" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="542" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="543" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="544" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="545" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="546" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="547" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="548" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="549" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="550" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="551" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="552" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="553" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="554" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="555" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="556" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="557" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="558" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="559" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="560" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="561" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="562" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="563" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="564" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="565" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="566" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="567" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="568" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="569" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="570" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="571" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="572" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="573" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="574" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="575" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="576" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="577" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="578" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="579" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="580" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="581" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="582" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="583" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="584" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="585" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="586" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="587" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="588" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="589" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="590" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="591" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="592" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="593" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="594" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="595" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="596" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="597" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="598" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="599" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="600" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="601" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="602" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="603" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="604" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="605" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="606" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="607" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="608" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="609" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="610" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="611" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="612" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="613" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="614" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="615" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="616" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="617" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="618" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="619" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="620" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="621" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="622" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="623" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="624" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="625" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="626" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="627" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="628" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="629" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="630" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="631" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="632" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="633" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="634" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="635" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="636" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="637" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="638" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="639" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="640" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="641" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="642" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="643" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="644" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="645" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="646" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="647" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="648" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="649" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="650" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="651" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="652" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="653" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="654" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="655" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="656" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="657" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="658" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="659" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="660" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="661" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="662" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="663" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="664" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="665" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="666" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="667" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="668" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="669" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="670" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="671" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="672" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="673" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="674" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="675" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="676" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="677" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="678" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="679" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="680" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="681" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="682" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="683" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="684" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="685" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="686" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="687" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="688" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="689" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="690" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="691" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="692" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="693" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="694" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="695" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="696" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="697" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="698" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="699" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="700" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="701" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="702" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="703" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="704" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="705" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="706" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="707" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="708" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="709" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="710" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="711" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="712" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="713" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="714" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="715" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="716" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="717" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="718" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="719" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="720" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="721" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="722" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="723" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="724" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="725" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="726" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="727" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="728" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="729" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="730" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="731" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="732" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="733" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1458,7 +5232,7 @@
       <c r="F2" s="10">
         <v>80</v>
       </c>
-      <c r="G2" t="s" s="62">
+      <c r="G2" t="s" s="691">
         <v>55</v>
       </c>
     </row>
@@ -1481,7 +5255,7 @@
       <c r="F3" s="10">
         <v>70</v>
       </c>
-      <c r="G3" t="s" s="63">
+      <c r="G3" t="s" s="692">
         <v>55</v>
       </c>
     </row>
@@ -1504,7 +5278,7 @@
       <c r="F4" s="10">
         <v>85</v>
       </c>
-      <c r="G4" t="s" s="64">
+      <c r="G4" t="s" s="693">
         <v>55</v>
       </c>
     </row>
@@ -1527,7 +5301,7 @@
       <c r="F5" s="10">
         <v>65</v>
       </c>
-      <c r="G5" t="s" s="65">
+      <c r="G5" t="s" s="694">
         <v>55</v>
       </c>
     </row>
@@ -1550,7 +5324,7 @@
       <c r="F6" s="10">
         <v>50</v>
       </c>
-      <c r="G6" t="s" s="66">
+      <c r="G6" t="s" s="695">
         <v>55</v>
       </c>
     </row>
@@ -1573,7 +5347,7 @@
       <c r="F7" s="10">
         <v>60</v>
       </c>
-      <c r="G7" t="s" s="67">
+      <c r="G7" t="s" s="696">
         <v>55</v>
       </c>
     </row>
@@ -1596,7 +5370,7 @@
       <c r="F8" s="10">
         <v>50</v>
       </c>
-      <c r="G8" t="s" s="68">
+      <c r="G8" t="s" s="697">
         <v>55</v>
       </c>
     </row>
@@ -1619,7 +5393,7 @@
       <c r="F9" s="10">
         <v>68</v>
       </c>
-      <c r="G9" t="s" s="69">
+      <c r="G9" t="s" s="698">
         <v>55</v>
       </c>
     </row>
@@ -1642,7 +5416,7 @@
       <c r="F10" s="10">
         <v>84</v>
       </c>
-      <c r="G10" t="s" s="70">
+      <c r="G10" t="s" s="699">
         <v>55</v>
       </c>
     </row>
@@ -1665,7 +5439,7 @@
       <c r="F11" s="10">
         <v>60</v>
       </c>
-      <c r="G11" t="s" s="71">
+      <c r="G11" t="s" s="700">
         <v>55</v>
       </c>
     </row>
@@ -1688,7 +5462,7 @@
       <c r="F12" s="10">
         <v>72</v>
       </c>
-      <c r="G12" t="s" s="72">
+      <c r="G12" t="s" s="701">
         <v>55</v>
       </c>
     </row>
@@ -1711,7 +5485,7 @@
       <c r="F13" s="10">
         <v>56</v>
       </c>
-      <c r="G13" t="s" s="73">
+      <c r="G13" t="s" s="702">
         <v>55</v>
       </c>
     </row>
@@ -1734,7 +5508,7 @@
       <c r="F14" s="10">
         <v>50</v>
       </c>
-      <c r="G14" t="s" s="74">
+      <c r="G14" t="s" s="703">
         <v>55</v>
       </c>
     </row>
@@ -1757,7 +5531,7 @@
       <c r="F15" s="10">
         <v>70</v>
       </c>
-      <c r="G15" t="s" s="75">
+      <c r="G15" t="s" s="704">
         <v>55</v>
       </c>
     </row>
@@ -1780,7 +5554,7 @@
       <c r="F16" s="10">
         <v>50</v>
       </c>
-      <c r="G16" t="s" s="76">
+      <c r="G16" t="s" s="705">
         <v>55</v>
       </c>
     </row>
@@ -1803,7 +5577,7 @@
       <c r="F17" s="10">
         <v>50</v>
       </c>
-      <c r="G17" t="s" s="77">
+      <c r="G17" t="s" s="706">
         <v>55</v>
       </c>
     </row>
@@ -1826,7 +5600,7 @@
       <c r="F18" s="10">
         <v>68</v>
       </c>
-      <c r="G18" t="s" s="78">
+      <c r="G18" t="s" s="707">
         <v>55</v>
       </c>
     </row>
@@ -1849,7 +5623,7 @@
       <c r="F19" s="10">
         <v>68</v>
       </c>
-      <c r="G19" t="s" s="79">
+      <c r="G19" t="s" s="708">
         <v>55</v>
       </c>
     </row>
@@ -1872,7 +5646,7 @@
       <c r="F20" s="10">
         <v>80</v>
       </c>
-      <c r="G20" t="s" s="80">
+      <c r="G20" t="s" s="709">
         <v>55</v>
       </c>
     </row>
@@ -1895,7 +5669,7 @@
       <c r="F21" s="10">
         <v>50</v>
       </c>
-      <c r="G21" t="s" s="81">
+      <c r="G21" t="s" s="710">
         <v>55</v>
       </c>
     </row>
@@ -1918,7 +5692,7 @@
       <c r="F22" s="10">
         <v>58</v>
       </c>
-      <c r="G22" t="s" s="82">
+      <c r="G22" t="s" s="711">
         <v>55</v>
       </c>
     </row>
@@ -1941,7 +5715,7 @@
       <c r="F23" s="10">
         <v>73</v>
       </c>
-      <c r="G23" t="s" s="83">
+      <c r="G23" t="s" s="712">
         <v>55</v>
       </c>
     </row>
@@ -1964,7 +5738,7 @@
       <c r="F24" s="10">
         <v>85</v>
       </c>
-      <c r="G24" t="s" s="84">
+      <c r="G24" t="s" s="713">
         <v>55</v>
       </c>
     </row>
@@ -2042,7 +5816,7 @@
       <c r="G2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H2" t="s" s="85">
+      <c r="H2" t="s" s="714">
         <v>55</v>
       </c>
     </row>
@@ -2068,7 +5842,7 @@
       <c r="G3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H3" t="s" s="86">
+      <c r="H3" t="s" s="715">
         <v>55</v>
       </c>
     </row>
@@ -2094,7 +5868,7 @@
       <c r="G4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H4" t="s" s="87">
+      <c r="H4" t="s" s="716">
         <v>55</v>
       </c>
     </row>
@@ -2120,7 +5894,7 @@
       <c r="G5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H5" t="s" s="88">
+      <c r="H5" t="s" s="717">
         <v>56</v>
       </c>
     </row>
@@ -2146,7 +5920,7 @@
       <c r="G6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H6" t="s" s="89">
+      <c r="H6" t="s" s="718">
         <v>55</v>
       </c>
     </row>
@@ -2172,7 +5946,7 @@
       <c r="G7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H7" t="s" s="90">
+      <c r="H7" t="s" s="719">
         <v>55</v>
       </c>
     </row>
@@ -2198,7 +5972,7 @@
       <c r="G8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H8" t="s" s="91">
+      <c r="H8" t="s" s="720">
         <v>55</v>
       </c>
     </row>
@@ -2224,7 +5998,7 @@
       <c r="G9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H9" t="s" s="92">
+      <c r="H9" t="s" s="721">
         <v>55</v>
       </c>
     </row>
@@ -2250,7 +6024,7 @@
       <c r="G10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H10" t="s" s="93">
+      <c r="H10" t="s" s="722">
         <v>55</v>
       </c>
     </row>
@@ -2276,7 +6050,7 @@
       <c r="G11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H11" t="s" s="94">
+      <c r="H11" t="s" s="723">
         <v>55</v>
       </c>
     </row>
@@ -2302,7 +6076,7 @@
       <c r="G12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H12" t="s" s="95">
+      <c r="H12" t="s" s="724">
         <v>55</v>
       </c>
     </row>
@@ -2328,7 +6102,7 @@
       <c r="G13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H13" t="s" s="96">
+      <c r="H13" t="s" s="725">
         <v>55</v>
       </c>
     </row>
@@ -2354,7 +6128,7 @@
       <c r="G14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H14" t="s" s="97">
+      <c r="H14" t="s" s="726">
         <v>56</v>
       </c>
     </row>
@@ -2378,7 +6152,7 @@
       <c r="G15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H15" t="s" s="98">
+      <c r="H15" t="s" s="727">
         <v>55</v>
       </c>
     </row>
@@ -2404,7 +6178,7 @@
       <c r="G16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H16" t="s" s="99">
+      <c r="H16" t="s" s="728">
         <v>55</v>
       </c>
     </row>
@@ -2430,7 +6204,7 @@
       <c r="G17" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H17" t="s" s="100">
+      <c r="H17" t="s" s="729">
         <v>55</v>
       </c>
     </row>
@@ -2456,7 +6230,7 @@
       <c r="G18" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H18" t="s" s="101">
+      <c r="H18" t="s" s="730">
         <v>55</v>
       </c>
     </row>
@@ -2482,7 +6256,7 @@
       <c r="G19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H19" t="s" s="102">
+      <c r="H19" t="s" s="731">
         <v>55</v>
       </c>
     </row>
@@ -2508,7 +6282,7 @@
       <c r="G20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H20" t="s" s="103">
+      <c r="H20" t="s" s="732">
         <v>55</v>
       </c>
     </row>
@@ -2534,7 +6308,7 @@
       <c r="G21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H21" t="s" s="104">
+      <c r="H21" t="s" s="733">
         <v>55</v>
       </c>
     </row>
@@ -2558,7 +6332,7 @@
       <c r="G22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H22" t="s" s="105">
+      <c r="H22" t="s" s="734">
         <v>55</v>
       </c>
     </row>
@@ -2584,7 +6358,7 @@
       <c r="G23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H23" t="s" s="106">
+      <c r="H23" t="s" s="735">
         <v>55</v>
       </c>
     </row>
@@ -2610,7 +6384,7 @@
       <c r="G24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H24" t="s" s="107">
+      <c r="H24" t="s" s="736">
         <v>55</v>
       </c>
     </row>
@@ -2636,7 +6410,7 @@
       <c r="G25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H25" t="s" s="108">
+      <c r="H25" t="s" s="737">
         <v>55</v>
       </c>
     </row>
@@ -2662,7 +6436,7 @@
       <c r="G26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H26" t="s" s="109">
+      <c r="H26" t="s" s="738">
         <v>55</v>
       </c>
     </row>
@@ -2688,7 +6462,7 @@
       <c r="G27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H27" t="s" s="110">
+      <c r="H27" t="s" s="739">
         <v>55</v>
       </c>
     </row>
@@ -2712,7 +6486,7 @@
       <c r="G28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H28" t="s" s="111">
+      <c r="H28" t="s" s="740">
         <v>55</v>
       </c>
     </row>

</xml_diff>